<commit_message>
Added analysis results of gender detection
</commit_message>
<xml_diff>
--- a/analysis-data/gender-detection/gender-detection-results.xlsx
+++ b/analysis-data/gender-detection/gender-detection-results.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -625,18 +625,6 @@
   <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -686,13 +674,25 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1103,11 +1103,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2126152456"/>
-        <c:axId val="2113947848"/>
+        <c:axId val="2090954168"/>
+        <c:axId val="2090951032"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126152456"/>
+        <c:axId val="2090954168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1116,7 +1116,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113947848"/>
+        <c:crossAx val="2090951032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1124,7 +1124,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113947848"/>
+        <c:axId val="2090951032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1146,7 +1146,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2126152456"/>
+        <c:crossAx val="2090954168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1547,261 +1547,261 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="42"/>
+      <c r="F1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="39"/>
+      <c r="H1" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="43"/>
+      <c r="J1" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="3" t="s">
+      <c r="K1" s="39"/>
+      <c r="L1" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="5"/>
+      <c r="M1" s="39"/>
     </row>
     <row r="2" spans="1:13" ht="16" thickBot="1">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="7" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="15">
         <v>5062</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="16">
         <f>B3/$E$9</f>
         <v>0.25309999999999999</v>
       </c>
-      <c r="D3" s="21">
+      <c r="D3" s="17">
         <v>4144</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="18">
         <f>D3/$E$9</f>
         <v>0.2072</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="19">
         <v>4892</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="16">
         <f>F3/$E$9</f>
         <v>0.24460000000000001</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="20">
         <v>4213</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="18">
         <f>H3/$E$9</f>
         <v>0.21065</v>
       </c>
-      <c r="J3" s="23">
+      <c r="J3" s="19">
         <v>6235</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="16">
         <f>J3/$E$9</f>
         <v>0.31175000000000003</v>
       </c>
-      <c r="L3" s="24">
+      <c r="L3" s="20">
         <v>5774</v>
       </c>
-      <c r="M3" s="25">
+      <c r="M3" s="21">
         <f>L3/$E$9</f>
         <v>0.28870000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="15">
         <v>4418</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="16">
         <f>B4/$E$9</f>
         <v>0.22090000000000001</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="17">
         <v>5880</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="18">
         <f>D4/$E$9</f>
         <v>0.29399999999999998</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="19">
         <v>3895</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="16">
         <f>F4/$E$9</f>
         <v>0.19475000000000001</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="20">
         <v>4791</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="18">
         <f>H4/$E$9</f>
         <v>0.23955000000000001</v>
       </c>
-      <c r="J4" s="23">
+      <c r="J4" s="19">
         <v>5769</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4" s="16">
         <f>J4/$E$9</f>
         <v>0.28844999999999998</v>
       </c>
-      <c r="L4" s="24">
+      <c r="L4" s="20">
         <v>8111</v>
       </c>
-      <c r="M4" s="25">
+      <c r="M4" s="21">
         <f>L4/$E$9</f>
         <v>0.40555000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="15">
         <v>85</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="16">
         <f>B5/$E$9</f>
         <v>4.2500000000000003E-3</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="17">
         <v>74</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="18">
         <f>D5/$E$9</f>
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="19">
         <v>3553</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="16">
         <f>F5/$E$9</f>
         <v>0.17765</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="20">
         <v>3412</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="18">
         <f>H5/$E$9</f>
         <v>0.1706</v>
       </c>
-      <c r="J5" s="23">
+      <c r="J5" s="19">
         <v>161</v>
       </c>
-      <c r="K5" s="20">
+      <c r="K5" s="16">
         <f>J5/$E$9</f>
         <v>8.0499999999999999E-3</v>
       </c>
-      <c r="L5" s="24">
+      <c r="L5" s="20">
         <v>158</v>
       </c>
-      <c r="M5" s="25">
+      <c r="M5" s="21">
         <f>L5/$E$9</f>
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="16" thickBot="1">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="22">
         <f>$E$9-SUM(B3:B5)</f>
         <v>10435</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="23">
         <f>B6/$E$9</f>
         <v>0.52175000000000005</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="24">
         <f>$E$9-SUM(D3:D5)</f>
         <v>9902</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="25">
         <f>D6/$E$9</f>
         <v>0.49509999999999998</v>
       </c>
-      <c r="F6" s="30">
+      <c r="F6" s="26">
         <f>$E$9-SUM(F3:F5)</f>
         <v>7660</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="23">
         <f>F6/$E$9</f>
         <v>0.38300000000000001</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="24">
         <f>$E$9-SUM(H3:H5)</f>
         <v>7584</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="25">
         <f>H6/$E$9</f>
         <v>0.37919999999999998</v>
       </c>
-      <c r="J6" s="30">
+      <c r="J6" s="26">
         <f>$E$9-SUM(J3:J5)</f>
         <v>7835</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="23">
         <f>J6/$E$9</f>
         <v>0.39174999999999999</v>
       </c>
-      <c r="L6" s="28">
+      <c r="L6" s="24">
         <f>$E$9-SUM(L3:L5)</f>
         <v>5957</v>
       </c>
-      <c r="M6" s="31">
+      <c r="M6" s="27">
         <f>L6/$E$9</f>
         <v>0.29785</v>
       </c>
@@ -1814,12 +1814,12 @@
     </row>
     <row r="9" spans="1:13" ht="19" thickBot="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43">
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="37">
         <v>20000</v>
       </c>
     </row>
@@ -1831,153 +1831,152 @@
     </row>
     <row r="12" spans="1:13" ht="16" thickBot="1">
       <c r="A12" s="1"/>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="17" t="s">
+      <c r="E12" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="32">
+      <c r="B13" s="28">
         <f>B3/$E$9</f>
         <v>0.25309999999999999</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="29">
         <f>D3/$E$9</f>
         <v>0.2072</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="29">
         <f>F3/$E$9</f>
         <v>0.24460000000000001</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="29">
         <f>H3/$E$9</f>
         <v>0.21065</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="29">
         <f>J3/$E$9</f>
         <v>0.31175000000000003</v>
       </c>
-      <c r="G13" s="34">
+      <c r="G13" s="30">
         <f>L3/$E$9</f>
         <v>0.28870000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="35">
+      <c r="B14" s="31">
         <f>B4/$E$9</f>
         <v>0.22090000000000001</v>
       </c>
-      <c r="C14" s="36">
+      <c r="C14" s="32">
         <f>D4/$E$9</f>
         <v>0.29399999999999998</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="32">
         <f>F4/$E$9</f>
         <v>0.19475000000000001</v>
       </c>
-      <c r="E14" s="36">
+      <c r="E14" s="32">
         <f>H4/$E$9</f>
         <v>0.23955000000000001</v>
       </c>
-      <c r="F14" s="36">
+      <c r="F14" s="32">
         <f>J4/$E$9</f>
         <v>0.28844999999999998</v>
       </c>
-      <c r="G14" s="37">
+      <c r="G14" s="33">
         <f>L4/$E$9</f>
         <v>0.40555000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="35">
+      <c r="B15" s="31">
         <f>B5/$E$9</f>
         <v>4.2500000000000003E-3</v>
       </c>
-      <c r="C15" s="36">
+      <c r="C15" s="32">
         <f>D5/$E$9</f>
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="D15" s="36">
+      <c r="D15" s="32">
         <f>F5/$E$9</f>
         <v>0.17765</v>
       </c>
-      <c r="E15" s="36">
+      <c r="E15" s="32">
         <f>H5/$E$9</f>
         <v>0.1706</v>
       </c>
-      <c r="F15" s="36">
+      <c r="F15" s="32">
         <f>J5/$E$9</f>
         <v>8.0499999999999999E-3</v>
       </c>
-      <c r="G15" s="37">
+      <c r="G15" s="33">
         <f>L5/$E$9</f>
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="16" thickBot="1">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="38">
+      <c r="B16" s="34">
         <f>B6/$E$9</f>
         <v>0.52175000000000005</v>
       </c>
-      <c r="C16" s="39">
+      <c r="C16" s="35">
         <f>D6/$E$9</f>
         <v>0.49509999999999998</v>
       </c>
-      <c r="D16" s="39">
+      <c r="D16" s="35">
         <f>F6/$E$9</f>
         <v>0.38300000000000001</v>
       </c>
-      <c r="E16" s="39">
+      <c r="E16" s="35">
         <f>H6/$E$9</f>
         <v>0.37919999999999998</v>
       </c>
-      <c r="F16" s="39">
+      <c r="F16" s="35">
         <f>J6/$E$9</f>
         <v>0.39174999999999999</v>
       </c>
-      <c r="G16" s="40">
+      <c r="G16" s="36">
         <f>L6/$E$9</f>
         <v>0.29785</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B1:C1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="H1:I1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Add gender detection document, and some adiitional changes
</commit_message>
<xml_diff>
--- a/analysis-data/gender-detection/gender-detection-results.xlsx
+++ b/analysis-data/gender-detection/gender-detection-results.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Precission and Recall" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Males</t>
   </si>
@@ -76,6 +77,45 @@
   </si>
   <si>
     <t>Sample (no. Twitter users):</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Negative cases</t>
+  </si>
+  <si>
+    <t>Positive cases</t>
+  </si>
+  <si>
+    <t>Predicted Negative</t>
+  </si>
+  <si>
+    <t>Predicted Postiive</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>True positive 294</t>
+  </si>
+  <si>
+    <t>True negative 194</t>
+  </si>
+  <si>
+    <t>False positive 100</t>
+  </si>
+  <si>
+    <t>False negative 412</t>
   </si>
 </sst>
 </file>
@@ -527,7 +567,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -621,8 +661,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -677,10 +753,13 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -692,11 +771,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="129">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -743,6 +820,24 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -789,6 +884,24 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1103,11 +1216,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="2090954168"/>
-        <c:axId val="2090951032"/>
+        <c:axId val="2077340488"/>
+        <c:axId val="2076719144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2090954168"/>
+        <c:axId val="2077340488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1116,7 +1229,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090951032"/>
+        <c:crossAx val="2076719144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1124,7 +1237,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2090951032"/>
+        <c:axId val="2076719144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1146,7 +1259,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2090954168"/>
+        <c:crossAx val="2077340488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1546,34 +1659,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="40" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="39"/>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="38" t="s">
+      <c r="E1" s="43"/>
+      <c r="F1" s="40" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="39"/>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="43"/>
-      <c r="J1" s="38" t="s">
+      <c r="I1" s="38"/>
+      <c r="J1" s="40" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="39"/>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="38" t="s">
         <v>4</v>
       </c>
       <c r="M1" s="39"/>
@@ -1814,11 +1927,11 @@
     </row>
     <row r="9" spans="1:13" ht="19" thickBot="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
       <c r="E9" s="37">
         <v>20000</v>
       </c>
@@ -1984,4 +2097,130 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="44">
+        <f>(F3+G4)/B15</f>
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="44">
+        <f>G4/(G4+F4)</f>
+        <v>0.41643059490084988</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3">
+        <f>B9</f>
+        <v>194</v>
+      </c>
+      <c r="G3">
+        <f>B10</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="44">
+        <f>G4/(G4+G3)</f>
+        <v>0.74619289340101524</v>
+      </c>
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4">
+        <f>B11</f>
+        <v>412</v>
+      </c>
+      <c r="G4">
+        <f>B8</f>
+        <v>294</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <f>SUM(B8:B11)</f>
+        <v>1000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>